<commit_message>
Combined all branch in delete functionality.
</commit_message>
<xml_diff>
--- a/DetailsFile/DetailsFile.xlsx
+++ b/DetailsFile/DetailsFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="21525" windowHeight="3990"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="28155" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Live branch</t>
   </si>
@@ -55,27 +55,9 @@
     <t>deptName</t>
   </si>
   <si>
-    <t>Station Name 1</t>
-  </si>
-  <si>
     <t>Andrew Department</t>
   </si>
   <si>
-    <t>//a[@href=\"http://live.retteralarm.de/admin/Informations/index\"]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle mail id </t>
-  </si>
-  <si>
-    <t xml:space="preserve">St 06 resource name </t>
-  </si>
-  <si>
-    <t>ADST06R2</t>
-  </si>
-  <si>
-    <t>Bhupesh+adst06v31</t>
-  </si>
-  <si>
     <t>bhupesh.dept_dev@atpl.in</t>
   </si>
   <si>
@@ -83,13 +65,37 @@
   </si>
   <si>
     <t>Bhupesh department 1</t>
+  </si>
+  <si>
+    <t>06v1</t>
+  </si>
+  <si>
+    <t>St1V1</t>
+  </si>
+  <si>
+    <t>st1N</t>
+  </si>
+  <si>
+    <t>06v3</t>
+  </si>
+  <si>
+    <t>St1V2</t>
+  </si>
+  <si>
+    <t>bh1st1</t>
+  </si>
+  <si>
+    <t>bh1st1&gt;1</t>
+  </si>
+  <si>
+    <t>bh1st1&gt;2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +109,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000C0"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +141,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,15 +489,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -490,49 +506,55 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="Bhupesh+adst06v31@atpl.in"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ntegration of live testing and development branch stage one is complete.
</commit_message>
<xml_diff>
--- a/DetailsFile/DetailsFile.xlsx
+++ b/DetailsFile/DetailsFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19410" windowHeight="10830"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23085" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Live branch</t>
   </si>
@@ -113,19 +113,51 @@
   </si>
   <si>
     <t>dailyVehicleEmailId2</t>
+  </si>
+  <si>
+    <t>914-IN-U11-U011-1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Station04</t>
+  </si>
+  <si>
+    <t>04v1</t>
+  </si>
+  <si>
+    <t>04v2</t>
+  </si>
+  <si>
+    <t>Station05</t>
+  </si>
+  <si>
+    <t>05v1</t>
+  </si>
+  <si>
+    <t>Bh1st2</t>
+  </si>
+  <si>
+    <t>st2v1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Source Sans Pro"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,8 +180,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +480,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -490,6 +523,9 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
@@ -509,6 +545,9 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
@@ -520,6 +559,9 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
@@ -531,6 +573,9 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
@@ -542,6 +587,9 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
@@ -553,6 +601,12 @@
       <c r="B9" t="s">
         <v>24</v>
       </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
@@ -560,6 +614,12 @@
       </c>
       <c r="B10" t="s">
         <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
combine testing and the live branch for adding firefighter, station user, and vehicle user.
</commit_message>
<xml_diff>
--- a/DetailsFile/DetailsFile.xlsx
+++ b/DetailsFile/DetailsFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23085" windowHeight="10845"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Live branch</t>
   </si>
@@ -140,13 +140,64 @@
   </si>
   <si>
     <t>st2v1</t>
+  </si>
+  <si>
+    <t>St1AttributeName</t>
+  </si>
+  <si>
+    <t>St1ResourceName</t>
+  </si>
+  <si>
+    <t>ADST06A2</t>
+  </si>
+  <si>
+    <t>ADST06R2</t>
+  </si>
+  <si>
+    <t>D1ST4A1</t>
+  </si>
+  <si>
+    <t>D1ST04R1</t>
+  </si>
+  <si>
+    <t>bhupesh+TestingStationUser1@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>bhupesh+TestingFirefighter1@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>bhupesh+TestingFirefighter2@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>stUEmail</t>
+  </si>
+  <si>
+    <t>ff1UEmail</t>
+  </si>
+  <si>
+    <t>ff2UEmail</t>
+  </si>
+  <si>
+    <t>bhupesh+LiveStationUser1@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>bhupesh+LiveFirefighter1@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>bhupesh+LiveFirefighter2@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>Bhupesh+d1St04V1newDaily@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>Bhupesh+d1St04V2newDaily@atinatechnology.in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +209,13 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Source Sans Pro"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,14 +235,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -477,16 +541,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -629,6 +693,9 @@
       <c r="B11" t="s">
         <v>29</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
@@ -636,6 +703,64 @@
       </c>
       <c r="B12" t="s">
         <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -644,9 +769,16 @@
     <hyperlink ref="D4" r:id="rId2"/>
     <hyperlink ref="B11" r:id="rId3"/>
     <hyperlink ref="B12" r:id="rId4"/>
+    <hyperlink ref="C15" r:id="rId5"/>
+    <hyperlink ref="C17" r:id="rId6"/>
+    <hyperlink ref="B15" r:id="rId7"/>
+    <hyperlink ref="B17" r:id="rId8"/>
+    <hyperlink ref="B16" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update-24 Dec 2024 -01
</commit_message>
<xml_diff>
--- a/DetailsFile/DetailsFile.xlsx
+++ b/DetailsFile/DetailsFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20220" windowHeight="10965"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18615" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Live branch</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Qwerty@123</t>
+  </si>
+  <si>
+    <t>bhupesh+DevStationUser1@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>BH1A1</t>
   </si>
 </sst>
 </file>
@@ -553,7 +559,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,6 +739,9 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
@@ -758,6 +767,9 @@
       <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
@@ -769,8 +781,11 @@
       <c r="C16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -778,6 +793,9 @@
         <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -796,9 +814,12 @@
     <hyperlink ref="D11" r:id="rId11"/>
     <hyperlink ref="D12" r:id="rId12"/>
     <hyperlink ref="D4" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update-24 Dec 2024 -02
</commit_message>
<xml_diff>
--- a/DetailsFile/DetailsFile.xlsx
+++ b/DetailsFile/DetailsFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Live branch</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>BH1A1</t>
+  </si>
+  <si>
+    <t>bhupesh+DevFirefighter1@atinatechnology.in</t>
+  </si>
+  <si>
+    <t>bhupesh+DevFirefighter2@atinatechnology.in</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -782,7 +788,7 @@
         <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -796,7 +802,7 @@
         <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>